<commit_message>
Updated Data Accession File
</commit_message>
<xml_diff>
--- a/Data Accessions.xlsx
+++ b/Data Accessions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toray.akcan/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96BC57C4-FD81-3548-8A92-FD54E40DF8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2589A000-72E2-F746-B4C6-45D13DA1EE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="2300" windowWidth="27640" windowHeight="16940" activeTab="4" xr2:uid="{C2A6E93C-E78D-484D-8FCF-6F97AE5ED66C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2271" uniqueCount="2093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="2100">
   <si>
     <t>Experiment</t>
   </si>
@@ -6315,6 +6315,27 @@
   </si>
   <si>
     <t>https://hgdownload.cse.ucsc.edu/goldenPath/hg19/database/cpgIslandExt.txt.gz</t>
+  </si>
+  <si>
+    <t>GENCODE Gene Annotations</t>
+  </si>
+  <si>
+    <t>http://ftp.ebi.ac.uk/pub/databases/gencode/Gencode_human/release_38/GRCh37_mapping/gencode.v38lift37.annotation.gff3.gz</t>
+  </si>
+  <si>
+    <t>GENCODE</t>
+  </si>
+  <si>
+    <t>GENCODE HGNC Metadata</t>
+  </si>
+  <si>
+    <t>http://ftp.ebi.ac.uk/pub/databases/gencode/Gencode_human/release_38/GRCh37_mapping/gencode.v38lift37.metadata.HGNC.gz</t>
+  </si>
+  <si>
+    <t>http://ftp.ebi.ac.uk/pub/databases/gencode/Gencode_human/release_38/GRCh37_mapping/gencode.v38lift37.metadata.RefSeq.gz</t>
+  </si>
+  <si>
+    <t>GENCODE RefSeq Metadata</t>
   </si>
 </sst>
 </file>
@@ -6341,6 +6362,7 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -17235,16 +17257,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{986228E0-55F3-5C40-ABF5-4B89AE96EA94}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="2" max="2" width="110.83203125" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17345,6 +17367,39 @@
       </c>
       <c r="C9" t="s">
         <v>2091</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2093</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2094</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2096</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2099</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>